<commit_message>
New shelter addresses with new column
</commit_message>
<xml_diff>
--- a/data/shelter_addresses.xlsx
+++ b/data/shelter_addresses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RachelClaireSilber/Desktop/R Project /sheltermap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB7F013-D286-9C48-B1BE-2178879BC38D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F553499-A24B-B045-9F9C-F3825E0B03EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="460" windowWidth="25060" windowHeight="15540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="460" windowWidth="25060" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LA" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="315">
   <si>
     <t>Name of Shelter or Supportive housing</t>
   </si>
@@ -2617,10 +2617,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -2632,11 +2632,12 @@
     <col min="5" max="5" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="91.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="91.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2658,11 +2659,11 @@
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>89</v>
       </c>
@@ -2685,10 +2686,13 @@
         <v>112</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>179</v>
       </c>
@@ -2711,10 +2715,13 @@
         <v>112</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>180</v>
       </c>
@@ -2737,10 +2744,13 @@
         <v>112</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>181</v>
       </c>
@@ -2763,10 +2773,13 @@
         <v>112</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>182</v>
       </c>
@@ -2789,10 +2802,13 @@
         <v>112</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>183</v>
       </c>
@@ -2815,10 +2831,13 @@
         <v>112</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>184</v>
       </c>
@@ -2841,10 +2860,13 @@
         <v>112</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -2867,10 +2889,13 @@
         <v>112</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
         <v>94</v>
       </c>
@@ -2893,10 +2918,13 @@
         <v>112</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>96</v>
       </c>
@@ -2919,10 +2947,13 @@
         <v>112</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
         <v>97</v>
       </c>
@@ -2945,10 +2976,13 @@
         <v>112</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
         <v>185</v>
       </c>
@@ -2971,10 +3005,13 @@
         <v>99</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
         <v>186</v>
       </c>
@@ -2997,10 +3034,13 @@
         <v>99</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
         <v>187</v>
       </c>
@@ -3023,10 +3063,13 @@
         <v>99</v>
       </c>
       <c r="H15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
         <v>188</v>
       </c>
@@ -3049,10 +3092,13 @@
         <v>99</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
         <v>101</v>
       </c>
@@ -3075,10 +3121,13 @@
         <v>111</v>
       </c>
       <c r="H17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
         <v>103</v>
       </c>
@@ -3101,10 +3150,13 @@
         <v>112</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
         <v>105</v>
       </c>
@@ -3127,10 +3179,13 @@
         <v>112</v>
       </c>
       <c r="H19" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
         <v>108</v>
       </c>
@@ -3153,10 +3208,13 @@
         <v>111</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
         <v>106</v>
       </c>
@@ -3179,10 +3237,13 @@
         <v>111</v>
       </c>
       <c r="H21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
         <v>107</v>
       </c>
@@ -3205,6 +3266,9 @@
         <v>111</v>
       </c>
       <c r="H22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3215,10 +3279,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -3230,11 +3294,12 @@
     <col min="5" max="5" width="9.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="89" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="5"/>
+    <col min="8" max="8" width="89" style="5" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3256,11 +3321,11 @@
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>189</v>
       </c>
@@ -3283,10 +3348,13 @@
         <v>165</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>191</v>
       </c>
@@ -3309,10 +3377,13 @@
         <v>165</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>192</v>
       </c>
@@ -3335,10 +3406,13 @@
         <v>165</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>193</v>
       </c>
@@ -3361,10 +3435,13 @@
         <v>165</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
         <v>194</v>
       </c>
@@ -3387,10 +3464,13 @@
         <v>110</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
         <v>83</v>
       </c>
@@ -3413,10 +3493,13 @@
         <v>110</v>
       </c>
       <c r="H7" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
         <v>196</v>
       </c>
@@ -3439,10 +3522,13 @@
         <v>203</v>
       </c>
       <c r="H8" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="5" t="s">
         <v>197</v>
       </c>
@@ -3465,10 +3551,13 @@
         <v>203</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="5" t="s">
         <v>198</v>
       </c>
@@ -3491,10 +3580,13 @@
         <v>203</v>
       </c>
       <c r="H10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
         <v>84</v>
       </c>
@@ -3517,10 +3609,13 @@
         <v>111</v>
       </c>
       <c r="H11" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
         <v>85</v>
       </c>
@@ -3543,10 +3638,13 @@
         <v>165</v>
       </c>
       <c r="H12" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="5" t="s">
         <v>86</v>
       </c>
@@ -3569,7 +3667,15 @@
         <v>165</v>
       </c>
       <c r="H13" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="H14" s="5" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3581,7 +3687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="64" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="64" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>

</xml_diff>